<commit_message>
IA-2841 mapping select multiple to boolean
</commit_message>
<xml_diff>
--- a/testdata/seed-data-command-cvs_survey.xlsx
+++ b/testdata/seed-data-command-cvs_survey.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="74">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -70,7 +70,43 @@
     <t xml:space="preserve">Statisfaction score</t>
   </si>
   <si>
+    <t xml:space="preserve">select_multiple reason</t>
+  </si>
+  <si>
+    <t xml:space="preserve">visit_reason</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reason of visits</t>
+  </si>
+  <si>
     <t xml:space="preserve">list name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reason</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pregnant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pregnant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">checkup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check-ups</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vaccination</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vaccination</t>
+  </si>
+  <si>
+    <t xml:space="preserve">malnutrition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Malnutrition</t>
   </si>
   <si>
     <t xml:space="preserve">title</t>
@@ -529,8 +565,8 @@
   </sheetPr>
   <dimension ref="A1:L1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.79296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -597,6 +633,17 @@
         <v>14</v>
       </c>
       <c r="F2" s="8"/>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="1048364" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048365" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -829,8 +876,8 @@
   </sheetPr>
   <dimension ref="A1:C1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.79296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -842,13 +889,57 @@
   <sheetData>
     <row r="1" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="1047452" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2007,18 +2098,18 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="12" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="13" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -2043,7 +2134,7 @@
       <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="4.66"/>
@@ -2056,125 +2147,125 @@
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="11" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="K8" s="0" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D10" s="14" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D11" s="14" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D12" s="14" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D13" s="15" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D14" s="15" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="0" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="0" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="0" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="0" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="1" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="J19" s="16" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F22" s="0" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G23" s="0" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G24" s="0" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J25" s="17" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F27" s="0" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="G27" s="0" t="s">
         <v>1</v>
@@ -2183,78 +2274,78 @@
         <v>2</v>
       </c>
       <c r="J27" s="0" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="K27" s="0" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G28" s="0" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="J28" s="0" t="n">
         <v>1</v>
       </c>
       <c r="K28" s="0" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="L28" s="18" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G29" s="0" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="J29" s="0" t="n">
         <v>2</v>
       </c>
       <c r="K29" s="0" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="L29" s="18" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G30" s="0" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="J30" s="0" t="n">
         <v>3</v>
       </c>
       <c r="K30" s="0" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="L30" s="18" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G31" s="0" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="J31" s="0" t="n">
         <v>4</v>
       </c>
       <c r="K31" s="0" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="L31" s="18" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>